<commit_message>
Changing the data format
</commit_message>
<xml_diff>
--- a/MAST-U_home.xlsx
+++ b/MAST-U_home.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianmarvell/Desktop/PYTHON/TOKAMAK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianmarvell/Desktop/PYTHON/TOKAMAK/LH-transition-MAST-U-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1685E86D-3CBA-1849-99B6-B8991BFEE1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1AA0A0-5BAA-994E-8659-7A36C88F106F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="1" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
   </bookViews>
   <sheets>
-    <sheet name="First_transistions" sheetId="1" r:id="rId1"/>
-    <sheet name="Second_transistions" sheetId="3" r:id="rId2"/>
+    <sheet name="transistions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>Divertor</t>
   </si>
@@ -107,9 +106,6 @@
     <t>Loop current [kA]</t>
   </si>
   <si>
-    <t>650??</t>
-  </si>
-  <si>
     <r>
       <t>B</t>
     </r>
@@ -130,12 +126,6 @@
       </rPr>
       <t>at magnetic axis [T]</t>
     </r>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>small</t>
   </si>
   <si>
     <r>
@@ -184,12 +174,6 @@
       </rPr>
       <t>ne</t>
     </r>
-  </si>
-  <si>
-    <t>850?</t>
-  </si>
-  <si>
-    <t>The plasma current dereases when HL transition occurs (I suggest dont plot this one)</t>
   </si>
   <si>
     <r>
@@ -319,7 +303,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +313,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,22 +341,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AADF9AE-A68A-514D-966F-61383FB2E8EB}">
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,66 +692,100 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
-    <col min="13" max="14" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="13" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:36" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="S1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="U1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Y1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="4"/>
+      <c r="AB1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>45154</v>
       </c>
@@ -784,32 +816,39 @@
       <c r="J2">
         <v>0.246</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="6">
+      <c r="K2" s="4">
+        <v>850</v>
+      </c>
+      <c r="L2" s="5">
         <v>0.52700000000000002</v>
       </c>
-      <c r="N2" s="6">
+      <c r="M2" s="5">
         <v>0.14299999999999999</v>
       </c>
-      <c r="O2" s="6">
+      <c r="N2" s="5">
         <v>0.89300000000000002</v>
       </c>
-      <c r="P2" s="6">
+      <c r="O2" s="5">
         <v>0.14299999999999999</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="P2" s="5">
         <v>0.249</v>
       </c>
-      <c r="R2" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>45312</v>
       </c>
@@ -840,29 +879,39 @@
       <c r="J3">
         <v>0.26500000000000001</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>12</v>
+      <c r="K3">
+        <v>721</v>
       </c>
       <c r="L3">
-        <v>721</v>
+        <v>3.5190000000000001</v>
       </c>
       <c r="M3">
-        <v>3.5190000000000001</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="N3">
+        <v>3.9809999999999999</v>
+      </c>
+      <c r="O3">
         <v>0.64100000000000001</v>
       </c>
-      <c r="O3">
-        <v>3.9809999999999999</v>
-      </c>
       <c r="P3">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="Q3">
         <v>0.26500000000000001</v>
       </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>45352</v>
       </c>
@@ -893,29 +942,39 @@
       <c r="J4">
         <v>0.26</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>12</v>
+      <c r="K4">
+        <v>611</v>
       </c>
       <c r="L4">
-        <v>611</v>
+        <v>1.3720000000000001</v>
       </c>
       <c r="M4">
-        <v>1.3720000000000001</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="N4">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="O4">
         <v>0.26800000000000002</v>
       </c>
-      <c r="O4">
-        <v>1.6679999999999999</v>
-      </c>
       <c r="P4">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="Q4">
         <v>0.30599999999999999</v>
       </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>45237</v>
       </c>
@@ -946,37 +1005,37 @@
       <c r="J5">
         <v>1.1180000000000001</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>12</v>
+      <c r="K5">
+        <v>502</v>
       </c>
       <c r="L5">
-        <v>502</v>
+        <v>2.4780000000000002</v>
       </c>
       <c r="M5">
-        <v>2.4780000000000002</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="N5">
+        <v>2.06</v>
+      </c>
+      <c r="O5">
         <v>0.41399999999999998</v>
       </c>
-      <c r="O5">
-        <v>2.06</v>
-      </c>
       <c r="P5">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="Q5">
         <v>1.8520000000000001</v>
       </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
@@ -984,9 +1043,8 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45475</v>
       </c>
@@ -1017,38 +1075,37 @@
       <c r="J6">
         <v>0.81799999999999995</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>12</v>
+      <c r="K6" s="1">
+        <v>280</v>
       </c>
       <c r="L6" s="1">
-        <v>280</v>
+        <v>1.135</v>
       </c>
       <c r="M6" s="1">
-        <v>1.135</v>
+        <v>0.123</v>
       </c>
       <c r="N6" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="O6" s="1">
         <v>0.123</v>
       </c>
-      <c r="O6" s="1">
-        <v>0.76200000000000001</v>
-      </c>
       <c r="P6" s="1">
-        <v>0.123</v>
-      </c>
-      <c r="Q6" s="1">
         <v>1.57</v>
       </c>
+      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
@@ -1056,9 +1113,8 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>45457</v>
       </c>
@@ -1089,396 +1145,34 @@
       <c r="J7">
         <v>0.76200000000000001</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41927764-DAAB-334C-94B7-23C8C1B6BE6A}">
-  <dimension ref="A1:S7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>45154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>45312</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>45352</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>45237</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>45475</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>750</v>
-      </c>
-      <c r="D6">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>45457</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>750</v>
-      </c>
-      <c r="D7">
-        <v>-0.55000000000000004</v>
-      </c>
-      <c r="E7">
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7">
         <v>316</v>
       </c>
-      <c r="F7">
+      <c r="R7">
         <v>1.0680000000000001</v>
       </c>
-      <c r="H7">
+      <c r="T7">
         <v>0.83599999999999997</v>
       </c>
-      <c r="J7">
+      <c r="V7">
         <v>0.99</v>
       </c>
-      <c r="L7">
+      <c r="X7">
         <v>902</v>
       </c>
-      <c r="M7">
+      <c r="Y7">
         <v>1.992</v>
       </c>
-      <c r="O7">
+      <c r="AA7">
         <v>1.6759999999999999</v>
       </c>
-      <c r="Q7">
+      <c r="AC7">
         <v>1.5840000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moving second set of transistions onto first sheet
</commit_message>
<xml_diff>
--- a/MAST-U_home.xlsx
+++ b/MAST-U_home.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianmarvell/Desktop/PYTHON/TOKAMAK/LH-transition-MAST-U-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C85CF3-B3E8-5E4B-88BC-C44CEAA211E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B736BD3-0F80-F740-8138-43F2DF3C6A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="transistions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Divertor</t>
   </si>
@@ -159,25 +159,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>SD</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>ne</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>n</t>
     </r>
     <r>
@@ -258,6 +239,9 @@
       </rPr>
       <t xml:space="preserve"> [MW]</t>
     </r>
+  </si>
+  <si>
+    <t>SET</t>
   </si>
 </sst>
 </file>
@@ -357,9 +341,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,146 +663,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AADF9AE-A68A-514D-966F-61383FB2E8EB}">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
-    <col min="12" max="13" width="11.83203125" customWidth="1"/>
+    <col min="1" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="14" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="8" t="s">
+      <c r="P1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>45154</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>600</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>848</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.628</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.159</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.98599999999999999</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.159</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.246</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -836,57 +799,60 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>45312</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>600</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>714</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.6070000000000002</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.48499999999999999</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3.0059999999999998</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.48499999999999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.26500000000000001</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>721</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>3.5190000000000001</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.64100000000000001</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3.9809999999999999</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.64100000000000001</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.26500000000000001</v>
       </c>
-      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -899,57 +865,60 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>45352</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>600</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>482</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.0820000000000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.20699999999999999</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.286</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.20699999999999999</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.26</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>611</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.3720000000000001</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.26800000000000002</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1.6679999999999999</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.26800000000000002</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.30599999999999999</v>
       </c>
-      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -962,57 +931,60 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>45237</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>600</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>312</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.82099999999999995</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.13200000000000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.075</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.13200000000000001</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1.1180000000000001</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>502</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2.06</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.41399999999999998</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2.4780000000000002</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.41399999999999998</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1.8520000000000001</v>
       </c>
-      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1025,145 +997,182 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
-      <c r="AD5" s="2"/>
+      <c r="AD5" s="1"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45475</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>750</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>198</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.90900000000000003</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.14599999999999999</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.127</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.14599999999999999</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.81799999999999995</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>280</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>0.76200000000000001</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>0.123</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>1.135</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>0.123</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>1.57</v>
       </c>
-      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="U6" s="1"/>
+      <c r="T6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AB6" s="1"/>
+      <c r="AA6" s="1"/>
       <c r="AC6" s="1"/>
-      <c r="AD6" s="2"/>
+      <c r="AD6" s="1"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>45457</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>750</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>204</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1.0509999999999999</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.16900000000000001</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.222</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.16900000000000001</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.76200000000000001</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="N7" s="3"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
-      <c r="Q7">
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>45457</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>750</v>
+      </c>
+      <c r="E8">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="F8">
         <v>316</v>
       </c>
-      <c r="R7">
+      <c r="G8">
         <v>0.83599999999999997</v>
       </c>
-      <c r="T7">
+      <c r="H8">
+        <f>0.135</f>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I8">
         <v>1.0680000000000001</v>
       </c>
-      <c r="V7">
+      <c r="J8">
+        <f>ROUND(I8*0.161,3)</f>
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="K8">
         <v>0.99</v>
       </c>
-      <c r="X7">
+      <c r="L8">
         <v>902</v>
       </c>
-      <c r="Y7">
+      <c r="M8">
         <v>1.6759999999999999</v>
       </c>
-      <c r="AA7">
+      <c r="N8">
+        <f>ROUND(M8*0.161,3)</f>
+        <v>0.27</v>
+      </c>
+      <c r="O8">
         <v>1.992</v>
       </c>
-      <c r="AC7">
+      <c r="P8">
+        <f>ROUND(O8*0.161,3)</f>
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="Q8">
         <v>1.5840000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="L8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding figures and raw data
</commit_message>
<xml_diff>
--- a/MAST-U_home.xlsx
+++ b/MAST-U_home.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hukaiyu/Desktop/UROP/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianmarvell/Desktop/PYTHON/TOKAMAK/LH-transition-MAST-U-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36A2467-DDDC-6A44-9086-8099BACC265C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572FB9CE-D8A7-9D4F-8670-340795D095B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{96CD2CCC-78D1-C142-B924-5DF05F92B3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="transistions" sheetId="1" r:id="rId1"/>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AADF9AE-A68A-514D-966F-61383FB2E8EB}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,10 +778,6 @@
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="1"/>
-      <c r="N2">
-        <f>+O2</f>
-        <v>0</v>
-      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>

</xml_diff>